<commit_message>
7-zip, allegro5 and Android Studio added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -178,6 +178,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -199,6 +200,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -255,7 +257,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -269,6 +271,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,7 +362,7 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -404,9 +410,9 @@
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -414,7 +420,7 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -422,7 +428,7 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -430,7 +436,7 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -438,7 +444,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -452,8 +458,8 @@
       <c r="A11" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,7 +468,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -470,7 +476,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -478,7 +484,7 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -486,7 +492,7 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -494,7 +500,7 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -502,23 +508,23 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -526,7 +532,7 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -534,7 +540,7 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -542,15 +548,15 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -566,7 +572,7 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -574,7 +580,7 @@
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -582,7 +588,7 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -590,7 +596,7 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -598,7 +604,7 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -606,31 +612,31 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -638,7 +644,7 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -646,7 +652,7 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -654,15 +660,15 @@
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
@@ -670,15 +676,15 @@
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="3"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
@@ -686,7 +692,7 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="4"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -694,23 +700,23 @@
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="5"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -718,7 +724,7 @@
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="4"/>
+      <c r="D44" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Virtualbox Guest Additions added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t xml:space="preserve">virtualbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">virtualbox-guest-additions</t>
   </si>
   <si>
     <t xml:space="preserve">visual-studio-2017-community</t>
@@ -359,10 +362,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -682,16 +685,16 @@
       <c r="A39" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,24 +710,32 @@
         <v>45</v>
       </c>
       <c r="B42" s="3"/>
-      <c r="C42" s="5"/>
+      <c r="C42" s="3"/>
       <c r="D42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="3"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="3"/>
       <c r="D44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
arduino and clementine added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -364,8 +364,8 @@
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,7 +431,7 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -439,7 +439,7 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">

</xml_diff>

<commit_message>
eyed3 and gimp added. preconfig updated to include pip3
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -365,7 +365,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,7 +447,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -471,7 +471,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">

</xml_diff>

<commit_message>
gitkraken added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -365,7 +365,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,7 +479,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">

</xml_diff>

<commit_message>
google-chrome added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -365,7 +365,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -487,7 +487,7 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">

</xml_diff>

<commit_message>
--ignorechecksum added for all Windows programs, path updated to use pip
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">youtube-dl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libreoffice</t>
   </si>
 </sst>
 </file>
@@ -362,10 +365,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -737,6 +740,14 @@
       <c r="C45" s="3"/>
       <c r="D45" s="5"/>
     </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
google-play-music-desktop-player added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -367,8 +367,8 @@
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -498,7 +498,7 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">

</xml_diff>

<commit_message>
kdenlive added for Manjaro
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t xml:space="preserve">libreoffice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kdenlive</t>
   </si>
 </sst>
 </file>
@@ -365,10 +368,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E48" activeCellId="0" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -748,13 +751,21 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="5"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ssh and okular added for Windows
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t xml:space="preserve">kdenlive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openssh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okular</t>
   </si>
 </sst>
 </file>
@@ -368,10 +374,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E48" activeCellId="0" sqref="E48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -759,13 +765,29 @@
       <c r="C47" s="3"/>
       <c r="D47" s="5"/>
     </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inkscape, krita and mysql-workbench added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -376,8 +376,8 @@
   </sheetPr>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,7 +515,7 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -523,7 +523,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -547,7 +547,7 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">

</xml_diff>

<commit_message>
netbeans, nuitka, prolog, pycharm-community added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -376,8 +376,8 @@
   </sheetPr>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -555,7 +555,7 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -563,7 +563,7 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="5"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -587,7 +587,7 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -595,7 +595,7 @@
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">

</xml_diff>

<commit_message>
python, python2 qbittorrent, racket added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -377,7 +377,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -603,7 +603,7 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="5"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -611,7 +611,7 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -619,7 +619,7 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -627,7 +627,7 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">

</xml_diff>

<commit_message>
soundconverter, steam added and preconfig updated for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t xml:space="preserve">rufus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remove-uneeded-dependencies</t>
   </si>
   <si>
     <t xml:space="preserve">soundconverter</t>
@@ -374,10 +371,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -643,15 +640,15 @@
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -674,7 +671,7 @@
         <v>39</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,31 +679,31 @@
         <v>40</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="5"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="5"/>
+      <c r="B39" s="3"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="3"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="5"/>
+      <c r="C40" s="3"/>
       <c r="D40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,22 +719,22 @@
         <v>45</v>
       </c>
       <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="3"/>
       <c r="D43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="5"/>
+      <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="5"/>
     </row>
@@ -746,23 +743,23 @@
         <v>48</v>
       </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="3"/>
       <c r="D46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,14 +769,6 @@
       <c r="B48" s="3"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
syncthing, unity3d added for Debian. mysql-workbench updated for Manjaro
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -373,8 +373,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -656,7 +656,7 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -664,7 +664,7 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -775,8 +775,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
virtualbox added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -373,8 +373,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -680,7 +680,7 @@
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">

</xml_diff>

<commit_message>
visual-studio-code added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -704,7 +704,7 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">

</xml_diff>

<commit_message>
libreoffice, okular added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -768,7 +768,7 @@
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="D48" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
vlc, woeusb added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -373,8 +373,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -712,7 +712,7 @@
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="5"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -728,7 +728,7 @@
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">

</xml_diff>

<commit_message>
kdenlive, ssh, youtube-dl added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -373,8 +373,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -736,7 +736,7 @@
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="5"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -752,7 +752,7 @@
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="5"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -760,7 +760,7 @@
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">

</xml_diff>

<commit_message>
lamp added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">okular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lamp</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,6 +294,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -371,10 +378,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D49" activeCellId="0" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -770,6 +777,14 @@
       <c r="C48" s="5"/>
       <c r="D48" s="3"/>
     </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="3"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
kivy added for Debian
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t xml:space="preserve">lamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kivy</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D49" activeCellId="0" sqref="D49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -785,6 +788,14 @@
       <c r="C49" s="6"/>
       <c r="D49" s="3"/>
     </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="3"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
google-chrome for Debian updated
libappindicator3-1 dependency added
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -383,11 +383,11 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>

</xml_diff>

<commit_message>
various Manjaro packages added, openssh fixed for Debian and Windows
kivy, libreoffice, okular, openssh, virtualbox-guest-additions added for Manjaro
openssh fixed for Debian
ssh name changed to openssh on Windows
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -383,8 +383,8 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -697,7 +697,7 @@
         <v>41</v>
       </c>
       <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,7 +753,7 @@
         <v>48</v>
       </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="5"/>
+      <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,7 +769,7 @@
         <v>50</v>
       </c>
       <c r="B47" s="3"/>
-      <c r="C47" s="5"/>
+      <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,7 +777,7 @@
         <v>51</v>
       </c>
       <c r="B48" s="3"/>
-      <c r="C48" s="5"/>
+      <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,7 +793,7 @@
         <v>53</v>
       </c>
       <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
+      <c r="C50" s="4"/>
       <c r="D50" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kivy added for Windows
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -383,8 +383,8 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -792,7 +792,7 @@
       <c r="A50" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="6"/>
+      <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="3"/>
     </row>

</xml_diff>

<commit_message>
soundkonverter added for Manjaro
</commit_message>
<xml_diff>
--- a/Scripts/Support Database.xlsx
+++ b/Scripts/Support Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -130,6 +130,9 @@
     <t xml:space="preserve">soundconverter</t>
   </si>
   <si>
+    <t xml:space="preserve">soundkonverter</t>
+  </si>
+  <si>
     <t xml:space="preserve">steam</t>
   </si>
   <si>
@@ -182,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">kivy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wamp</t>
   </si>
 </sst>
 </file>
@@ -381,10 +387,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -656,9 +662,9 @@
       <c r="A33" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -681,22 +687,22 @@
         <v>39</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
@@ -704,17 +710,17 @@
       <c r="A39" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -729,22 +735,22 @@
         <v>45</v>
       </c>
       <c r="B42" s="3"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="3"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
@@ -760,7 +766,7 @@
       <c r="A46" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="5"/>
+      <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
@@ -768,7 +774,7 @@
       <c r="A47" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="3"/>
+      <c r="B47" s="5"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
@@ -784,17 +790,33 @@
       <c r="A49" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
       <c r="D50" s="3"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>